<commit_message>
Refine rtl generation code
</commit_message>
<xml_diff>
--- a/docs/reg_test_plan.xlsx
+++ b/docs/reg_test_plan.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85002572-022A-44A7-975F-65CA3E775C61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEF43B1-4DD6-4E6D-9ACB-A545868813D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4992" yWindow="2760" windowWidth="22776" windowHeight="14652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,38 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="51">
-  <si>
-    <t>序号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>功能</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>写操作</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>具体描述</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg_mst内部写操作</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg_mst外部写操作，同时写入第一级reg_slv的内部</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg_mst外部写操作，同时写入第一级reg_slv的外部，第二级reg_slv内部</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>读操作</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="54">
   <si>
     <t>连续写</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -205,19 +174,63 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>APB操作</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>读写超时，看interrupt能否被拉起以及PSLVERR时序，同时clear能否清终端，以及内部相关状态机复位情况</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>decode验证</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>前后门访问比较</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>field sync reset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>同步复位信号是否能够复位相应field</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>decoder验证</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>APB写操作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>APB读操作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>APB读写超时</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>APB下发写请求，对regmst内部寄存器写操作，终端节点深度为1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>APB下发写请求，对regmst外部写操作，指向reg tree中regmst下第一级regslv的内部寄存器，终端节点深度为2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>APB下发写请求，对regmst外部写操作，指向reg tree中regmst下第二级regslv的内部寄存器，终端节点深度为3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>APB下发写请求，对regmst外部写操作，指向reg tree中regmst下第一级的外部memory，终端节点深度为2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试项目编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>描述</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -547,457 +560,364 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.9140625" style="1"/>
-    <col min="2" max="2" width="22.75" customWidth="1"/>
-    <col min="3" max="3" width="86.9140625" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.77734375" customWidth="1"/>
+    <col min="3" max="3" width="98.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="C19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" t="s">
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
+      <c r="C26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" t="s">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="C29" t="s">
         <v>23</v>
       </c>
-      <c r="C20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" t="s">
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" t="s">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="C33" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" t="s">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="C34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" t="s">
         <v>30</v>
       </c>
-      <c r="C27" t="s">
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="C38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="C39" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" t="s">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" t="s">
         <v>35</v>
       </c>
-      <c r="C31" t="s">
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="1">
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>35</v>
-      </c>
-      <c r="C32" t="s">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>40</v>
-      </c>
-      <c r="C36" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C37" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="1">
-        <v>39</v>
-      </c>
-      <c r="B40" t="s">
-        <v>40</v>
-      </c>
-      <c r="C40" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>